<commit_message>
- import deposit with type
</commit_message>
<xml_diff>
--- a/public/ClarkWell_Deposit_Import_Template.xlsx
+++ b/public/ClarkWell_Deposit_Import_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Tech\ClarkWell23Feb\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Tech\Clarkwell v2\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE6299F-9D46-4894-B04C-43B2EEB7A2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320A8FE9-6B56-42D2-AEDD-ACBD29F02F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3046B44F-C017-4D54-A8C2-A09887A012DA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>email</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>test@test.com</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>1(deposit), 2(withdraw)</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63F80D8-1B82-4EFF-8524-6476FADFFDFF}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,7 +431,7 @@
     <col min="4" max="4" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +441,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -445,6 +454,9 @@
       </c>
       <c r="C2">
         <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>